<commit_message>
updates to acceptance criteria and project brief as screenshot
</commit_message>
<xml_diff>
--- a/planning/Acceptance Criteria.xlsx
+++ b/planning/Acceptance Criteria.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52E7497D-AD28-4DE1-A426-DB3B31E4A38C}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianburgin/codeclan_work/week_09/project/w10_stocks_project/planning/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8574D984-8AFA-7947-B5BB-09BF883629AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="15780" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>acceptance criteria</t>
   </si>
@@ -66,13 +69,16 @@
   </si>
   <si>
     <t>Share is removed from portfolio</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,17 +485,17 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -500,102 +506,114 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" ht="30">
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="30">
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="30">
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="30">
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="30">
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>

</xml_diff>